<commit_message>
idk what i did
</commit_message>
<xml_diff>
--- a/BUSIN-PROJECT/data/new_cars_by_fuel_type.xlsx
+++ b/BUSIN-PROJECT/data/new_cars_by_fuel_type.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guust\Documents\GitHub\Business-Intelligence-Groep-5\BUSIN-PROJECT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EBC1DDC-CF46-4E30-B14B-0F84DD8E95A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1317BE-BFA0-4FA1-954D-911BE65A1C04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="83">
   <si>
     <t>New registrations of passenger cars by type of motor energy [ROAD_EQR_CARPDA__custom_180051]</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -414,10 +423,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -425,6 +430,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,22 +827,22 @@
       <c r="A8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1369,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J180"/>
+  <dimension ref="A1:J175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1389,10 +1398,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>77</v>
       </c>
       <c r="C1" s="13" t="s">
@@ -1416,7 +1425,7 @@
       <c r="I1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="17" t="s">
+      <c r="J1" s="15" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1430,7 +1439,9 @@
       <c r="C2" s="5">
         <v>169665</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E2" s="5">
         <v>319863</v>
       </c>
@@ -1446,7 +1457,7 @@
       <c r="I2" s="5">
         <v>231</v>
       </c>
-      <c r="J2" s="18">
+      <c r="J2" s="16">
         <f>SUM(C2:I2)</f>
         <v>491210</v>
       </c>
@@ -1461,7 +1472,9 @@
       <c r="C3" s="4">
         <v>181524</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E3" s="4">
         <v>303953</v>
       </c>
@@ -1477,7 +1490,7 @@
       <c r="I3" s="4">
         <v>804</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="16">
         <f t="shared" ref="J3:J66" si="0">SUM(C3:I3)</f>
         <v>489945</v>
       </c>
@@ -1510,7 +1523,7 @@
       <c r="I4" s="5">
         <v>646</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="16">
         <f t="shared" si="0"/>
         <v>508430</v>
       </c>
@@ -1543,7 +1556,7 @@
       <c r="I5" s="4">
         <v>1552</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="16">
         <f t="shared" si="0"/>
         <v>550549</v>
       </c>
@@ -1576,7 +1589,7 @@
       <c r="I6" s="5">
         <v>1958</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="16">
         <f t="shared" si="0"/>
         <v>559110</v>
       </c>
@@ -1609,7 +1622,7 @@
       <c r="I7" s="4">
         <v>2810</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="16">
         <f t="shared" si="0"/>
         <v>565011</v>
       </c>
@@ -1624,15 +1637,25 @@
       <c r="C8" s="5">
         <v>122644</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E8" s="5">
         <v>57435</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="18">
+      <c r="F8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" s="16">
         <f t="shared" si="0"/>
         <v>180079</v>
       </c>
@@ -1647,15 +1670,25 @@
       <c r="C9" s="4">
         <v>127172</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E9" s="4">
         <v>59544</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="18">
+      <c r="F9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" s="16">
         <f t="shared" si="0"/>
         <v>186716</v>
       </c>
@@ -1670,15 +1703,25 @@
       <c r="C10" s="5">
         <v>137698</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E10" s="5">
         <v>64203</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="18">
+      <c r="F10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" s="16">
         <f t="shared" si="0"/>
         <v>201901</v>
       </c>
@@ -1693,15 +1736,25 @@
       <c r="C11" s="4">
         <v>140371</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E11" s="4">
         <v>80216</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="18">
+      <c r="F11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" s="16">
         <f t="shared" si="0"/>
         <v>220587</v>
       </c>
@@ -1716,15 +1769,25 @@
       <c r="C12" s="5">
         <v>142607</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E12" s="5">
         <v>77495</v>
       </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="18">
+      <c r="F12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" s="16">
         <f t="shared" si="0"/>
         <v>220102</v>
       </c>
@@ -1739,15 +1802,25 @@
       <c r="C13" s="4">
         <v>141320</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E13" s="4">
         <v>72475</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="18">
+      <c r="F13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" s="16">
         <f t="shared" si="0"/>
         <v>213795</v>
       </c>
@@ -1780,7 +1853,7 @@
       <c r="I14" s="5">
         <v>26391</v>
       </c>
-      <c r="J14" s="18">
+      <c r="J14" s="16">
         <f t="shared" si="0"/>
         <v>2998965</v>
       </c>
@@ -1813,7 +1886,7 @@
       <c r="I15" s="4">
         <v>27532</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="16">
         <f t="shared" si="0"/>
         <v>3087255</v>
       </c>
@@ -1846,7 +1919,7 @@
       <c r="I16" s="5">
         <v>33838</v>
       </c>
-      <c r="J16" s="18">
+      <c r="J16" s="16">
         <f t="shared" si="0"/>
         <v>3262244</v>
       </c>
@@ -1879,7 +1952,7 @@
       <c r="I17" s="4">
         <v>48063</v>
       </c>
-      <c r="J17" s="18">
+      <c r="J17" s="16">
         <f t="shared" si="0"/>
         <v>3417293</v>
       </c>
@@ -1912,7 +1985,7 @@
       <c r="I18" s="5">
         <v>84819</v>
       </c>
-      <c r="J18" s="18">
+      <c r="J18" s="16">
         <f t="shared" si="0"/>
         <v>3559260</v>
       </c>
@@ -1945,7 +2018,7 @@
       <c r="I19" s="4">
         <v>130419</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="16">
         <f t="shared" si="0"/>
         <v>3617726</v>
       </c>
@@ -1978,7 +2051,7 @@
       <c r="I20" s="5">
         <v>0</v>
       </c>
-      <c r="J20" s="18">
+      <c r="J20" s="16">
         <f t="shared" si="0"/>
         <v>19827</v>
       </c>
@@ -2008,8 +2081,10 @@
       <c r="H21" s="4">
         <v>348</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="18">
+      <c r="I21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="16">
         <f t="shared" si="0"/>
         <v>21476</v>
       </c>
@@ -2039,8 +2114,10 @@
       <c r="H22" s="5">
         <v>46</v>
       </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="18">
+      <c r="I22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J22" s="16">
         <f t="shared" si="0"/>
         <v>21110</v>
       </c>
@@ -2070,8 +2147,10 @@
       <c r="H23" s="4">
         <v>35</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="18">
+      <c r="I23" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J23" s="16">
         <f t="shared" si="0"/>
         <v>23055</v>
       </c>
@@ -2101,8 +2180,10 @@
       <c r="H24" s="5">
         <v>35</v>
       </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="18">
+      <c r="I24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J24" s="16">
         <f t="shared" si="0"/>
         <v>25656</v>
       </c>
@@ -2132,8 +2213,10 @@
       <c r="H25" s="4">
         <v>86</v>
       </c>
-      <c r="I25" s="4"/>
-      <c r="J25" s="18">
+      <c r="I25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J25" s="16">
         <f t="shared" si="0"/>
         <v>26385</v>
       </c>
@@ -2145,14 +2228,28 @@
       <c r="B26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="18">
+      <c r="C26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J26" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2167,11 +2264,15 @@
       <c r="C27" s="4">
         <v>21067</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E27" s="4">
         <v>61917</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G27" s="4">
         <v>194</v>
       </c>
@@ -2181,7 +2282,7 @@
       <c r="I27" s="4">
         <v>958</v>
       </c>
-      <c r="J27" s="18">
+      <c r="J27" s="16">
         <f t="shared" si="0"/>
         <v>85288</v>
       </c>
@@ -2196,11 +2297,15 @@
       <c r="C28" s="5">
         <v>35311</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E28" s="5">
         <v>92436</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G28" s="5">
         <v>494</v>
       </c>
@@ -2210,7 +2315,7 @@
       <c r="I28" s="5">
         <v>1718</v>
       </c>
-      <c r="J28" s="18">
+      <c r="J28" s="16">
         <f t="shared" si="0"/>
         <v>132171</v>
       </c>
@@ -2225,11 +2330,15 @@
       <c r="C29" s="4">
         <v>41160</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E29" s="4">
         <v>105257</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G29" s="4">
         <v>402</v>
       </c>
@@ -2239,7 +2348,7 @@
       <c r="I29" s="4">
         <v>2944</v>
       </c>
-      <c r="J29" s="18">
+      <c r="J29" s="16">
         <f t="shared" si="0"/>
         <v>153109</v>
       </c>
@@ -2254,11 +2363,15 @@
       <c r="C30" s="5">
         <v>40798</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E30" s="5">
         <v>87640</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G30" s="5">
         <v>631</v>
       </c>
@@ -2268,7 +2381,7 @@
       <c r="I30" s="5">
         <v>4813</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="16">
         <f t="shared" si="0"/>
         <v>139326</v>
       </c>
@@ -2283,11 +2396,15 @@
       <c r="C31" s="4">
         <v>48840</v>
       </c>
-      <c r="D31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E31" s="4">
         <v>70732</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G31" s="4">
         <v>1252</v>
       </c>
@@ -2297,7 +2414,7 @@
       <c r="I31" s="4">
         <v>7725</v>
       </c>
-      <c r="J31" s="18">
+      <c r="J31" s="16">
         <f t="shared" si="0"/>
         <v>137526</v>
       </c>
@@ -2309,16 +2426,28 @@
       <c r="B32" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H32" s="5">
         <v>2088</v>
       </c>
-      <c r="I32" s="5"/>
-      <c r="J32" s="18">
+      <c r="I32" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J32" s="16">
         <f t="shared" si="0"/>
         <v>2088</v>
       </c>
@@ -2351,7 +2480,7 @@
       <c r="I33" s="4">
         <v>167</v>
       </c>
-      <c r="J33" s="18">
+      <c r="J33" s="16">
         <f t="shared" si="0"/>
         <v>892708</v>
       </c>
@@ -2384,7 +2513,7 @@
       <c r="I34" s="5">
         <v>36</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="16">
         <f t="shared" si="0"/>
         <v>1099289</v>
       </c>
@@ -2417,7 +2546,7 @@
       <c r="I35" s="4">
         <v>47</v>
       </c>
-      <c r="J35" s="18">
+      <c r="J35" s="16">
         <f t="shared" si="0"/>
         <v>1235415</v>
       </c>
@@ -2450,7 +2579,7 @@
       <c r="I36" s="5">
         <v>80</v>
       </c>
-      <c r="J36" s="18">
+      <c r="J36" s="16">
         <f t="shared" si="0"/>
         <v>1354655</v>
       </c>
@@ -2483,7 +2612,7 @@
       <c r="I37" s="4">
         <v>66</v>
       </c>
-      <c r="J37" s="18">
+      <c r="J37" s="16">
         <f t="shared" si="0"/>
         <v>1458698</v>
       </c>
@@ -2516,7 +2645,7 @@
       <c r="I38" s="5">
         <v>86</v>
       </c>
-      <c r="J38" s="18">
+      <c r="J38" s="16">
         <f t="shared" si="0"/>
         <v>1765839</v>
       </c>
@@ -2549,7 +2678,7 @@
       <c r="I39" s="4">
         <v>38</v>
       </c>
-      <c r="J39" s="18">
+      <c r="J39" s="16">
         <f t="shared" si="0"/>
         <v>1776487</v>
       </c>
@@ -2582,7 +2711,7 @@
       <c r="I40" s="5">
         <v>46</v>
       </c>
-      <c r="J40" s="18">
+      <c r="J40" s="16">
         <f t="shared" si="0"/>
         <v>1903590</v>
       </c>
@@ -2615,7 +2744,7 @@
       <c r="I41" s="4">
         <v>83</v>
       </c>
-      <c r="J41" s="18">
+      <c r="J41" s="16">
         <f t="shared" si="0"/>
         <v>2006369</v>
       </c>
@@ -2648,7 +2777,7 @@
       <c r="I42" s="5">
         <v>112</v>
       </c>
-      <c r="J42" s="18">
+      <c r="J42" s="16">
         <f t="shared" si="0"/>
         <v>2104609</v>
       </c>
@@ -2681,7 +2810,7 @@
       <c r="I43" s="4">
         <v>34</v>
       </c>
-      <c r="J43" s="18">
+      <c r="J43" s="16">
         <f t="shared" si="0"/>
         <v>2169600</v>
       </c>
@@ -2714,7 +2843,7 @@
       <c r="I44" s="5">
         <v>98</v>
       </c>
-      <c r="J44" s="18">
+      <c r="J44" s="16">
         <f t="shared" si="0"/>
         <v>46835</v>
       </c>
@@ -2747,7 +2876,7 @@
       <c r="I45" s="4">
         <v>420</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="16">
         <f t="shared" si="0"/>
         <v>69493</v>
       </c>
@@ -2762,11 +2891,15 @@
       <c r="C46" s="5">
         <v>16311</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E46" s="5">
         <v>56807</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="F46" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G46" s="5">
         <v>80</v>
       </c>
@@ -2776,7 +2909,7 @@
       <c r="I46" s="5">
         <v>466</v>
       </c>
-      <c r="J46" s="18">
+      <c r="J46" s="16">
         <f t="shared" si="0"/>
         <v>74727</v>
       </c>
@@ -2809,7 +2942,7 @@
       <c r="I47" s="4">
         <v>501</v>
       </c>
-      <c r="J47" s="18">
+      <c r="J47" s="16">
         <f t="shared" si="0"/>
         <v>97026</v>
       </c>
@@ -2824,7 +2957,9 @@
       <c r="C48" s="5">
         <v>20875</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E48" s="5">
         <v>71385</v>
       </c>
@@ -2840,7 +2975,7 @@
       <c r="I48" s="5">
         <v>664</v>
       </c>
-      <c r="J48" s="18">
+      <c r="J48" s="16">
         <f t="shared" si="0"/>
         <v>94522</v>
       </c>
@@ -2855,7 +2990,9 @@
       <c r="C49" s="4">
         <v>40964</v>
       </c>
-      <c r="D49" s="4"/>
+      <c r="D49" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E49" s="4">
         <v>97276</v>
       </c>
@@ -2871,7 +3008,7 @@
       <c r="I49" s="4">
         <v>1085</v>
       </c>
-      <c r="J49" s="18">
+      <c r="J49" s="16">
         <f t="shared" si="0"/>
         <v>141913</v>
       </c>
@@ -2895,14 +3032,16 @@
       <c r="F50" s="5">
         <v>67982</v>
       </c>
-      <c r="G50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H50" s="5">
         <v>184648</v>
       </c>
       <c r="I50" s="5">
         <v>828</v>
       </c>
-      <c r="J50" s="18">
+      <c r="J50" s="16">
         <f t="shared" si="0"/>
         <v>1495982</v>
       </c>
@@ -2914,22 +3053,28 @@
       <c r="B51" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="4"/>
+      <c r="C51" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="D51" s="4">
         <v>124092</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F51" s="4">
         <v>72387</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H51" s="4">
         <v>197582</v>
       </c>
       <c r="I51" s="4">
         <v>1103</v>
       </c>
-      <c r="J51" s="18">
+      <c r="J51" s="16">
         <f t="shared" si="0"/>
         <v>395164</v>
       </c>
@@ -2941,18 +3086,28 @@
       <c r="B52" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H52" s="5">
         <v>185333</v>
       </c>
       <c r="I52" s="5">
         <v>1467</v>
       </c>
-      <c r="J52" s="18">
+      <c r="J52" s="16">
         <f t="shared" si="0"/>
         <v>186800</v>
       </c>
@@ -2964,20 +3119,28 @@
       <c r="B53" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="D53" s="4">
         <v>101619</v>
       </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="E53" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H53" s="4">
         <v>146790</v>
       </c>
       <c r="I53" s="4">
         <v>1374</v>
       </c>
-      <c r="J53" s="18">
+      <c r="J53" s="16">
         <f t="shared" si="0"/>
         <v>249783</v>
       </c>
@@ -2989,22 +3152,28 @@
       <c r="B54" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="D54" s="5">
         <v>128765</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="F54" s="5">
         <v>32659</v>
       </c>
-      <c r="G54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H54" s="5">
         <v>163320</v>
       </c>
       <c r="I54" s="5">
         <v>1896</v>
       </c>
-      <c r="J54" s="18">
+      <c r="J54" s="16">
         <f t="shared" si="0"/>
         <v>326640</v>
       </c>
@@ -3016,22 +3185,28 @@
       <c r="B55" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="D55" s="4">
         <v>126778</v>
       </c>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F55" s="4">
         <v>37416</v>
       </c>
-      <c r="G55" s="4"/>
+      <c r="G55" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H55" s="4">
         <v>169133</v>
       </c>
       <c r="I55" s="4">
         <v>4939</v>
       </c>
-      <c r="J55" s="18">
+      <c r="J55" s="16">
         <f t="shared" si="0"/>
         <v>338266</v>
       </c>
@@ -3064,7 +3239,7 @@
       <c r="I56" s="5">
         <v>0</v>
       </c>
-      <c r="J56" s="18">
+      <c r="J56" s="16">
         <f t="shared" si="0"/>
         <v>14786</v>
       </c>
@@ -3097,7 +3272,7 @@
       <c r="I57" s="4">
         <v>0</v>
       </c>
-      <c r="J57" s="18">
+      <c r="J57" s="16">
         <f t="shared" si="0"/>
         <v>17942</v>
       </c>
@@ -3130,7 +3305,7 @@
       <c r="I58" s="5">
         <v>0</v>
       </c>
-      <c r="J58" s="18">
+      <c r="J58" s="16">
         <f t="shared" si="0"/>
         <v>21471</v>
       </c>
@@ -3163,7 +3338,7 @@
       <c r="I59" s="4">
         <v>0</v>
       </c>
-      <c r="J59" s="18">
+      <c r="J59" s="16">
         <f t="shared" si="0"/>
         <v>27978</v>
       </c>
@@ -3196,7 +3371,7 @@
       <c r="I60" s="5">
         <v>13</v>
       </c>
-      <c r="J60" s="18">
+      <c r="J60" s="16">
         <f t="shared" si="0"/>
         <v>36124</v>
       </c>
@@ -3229,7 +3404,7 @@
       <c r="I61" s="4">
         <v>9</v>
       </c>
-      <c r="J61" s="18">
+      <c r="J61" s="16">
         <f t="shared" si="0"/>
         <v>40720</v>
       </c>
@@ -3244,17 +3419,25 @@
       <c r="C62" s="5">
         <v>14293</v>
       </c>
-      <c r="D62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E62" s="5">
         <v>41502</v>
       </c>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
+      <c r="F62" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H62" s="5">
         <v>11</v>
       </c>
-      <c r="I62" s="5"/>
-      <c r="J62" s="18">
+      <c r="I62" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J62" s="16">
         <f t="shared" si="0"/>
         <v>55806</v>
       </c>
@@ -3287,7 +3470,7 @@
       <c r="I63" s="4">
         <v>211</v>
       </c>
-      <c r="J63" s="18">
+      <c r="J63" s="16">
         <f t="shared" si="0"/>
         <v>13769</v>
       </c>
@@ -3320,7 +3503,7 @@
       <c r="I64" s="5">
         <v>140</v>
       </c>
-      <c r="J64" s="18">
+      <c r="J64" s="16">
         <f t="shared" si="0"/>
         <v>14588</v>
       </c>
@@ -3353,7 +3536,7 @@
       <c r="I65" s="4">
         <v>0</v>
       </c>
-      <c r="J65" s="18">
+      <c r="J65" s="16">
         <f t="shared" si="0"/>
         <v>16868</v>
       </c>
@@ -3386,7 +3569,7 @@
       <c r="I66" s="5">
         <v>0</v>
       </c>
-      <c r="J66" s="18">
+      <c r="J66" s="16">
         <f t="shared" si="0"/>
         <v>17194</v>
       </c>
@@ -3419,7 +3602,7 @@
       <c r="I67" s="4">
         <v>0</v>
       </c>
-      <c r="J67" s="18">
+      <c r="J67" s="16">
         <f t="shared" ref="J67:J130" si="1">SUM(C67:I67)</f>
         <v>17323</v>
       </c>
@@ -3452,7 +3635,7 @@
       <c r="I68" s="5">
         <v>523</v>
       </c>
-      <c r="J68" s="18">
+      <c r="J68" s="16">
         <f t="shared" si="1"/>
         <v>156389</v>
       </c>
@@ -3485,7 +3668,7 @@
       <c r="I69" s="4">
         <v>692</v>
       </c>
-      <c r="J69" s="18">
+      <c r="J69" s="16">
         <f t="shared" si="1"/>
         <v>136857</v>
       </c>
@@ -3518,7 +3701,7 @@
       <c r="I70" s="5">
         <v>919</v>
       </c>
-      <c r="J70" s="18">
+      <c r="J70" s="16">
         <f t="shared" si="1"/>
         <v>133435</v>
       </c>
@@ -3551,7 +3734,7 @@
       <c r="I71" s="4">
         <v>2853</v>
       </c>
-      <c r="J71" s="18">
+      <c r="J71" s="16">
         <f t="shared" si="1"/>
         <v>142951</v>
       </c>
@@ -3584,7 +3767,7 @@
       <c r="I72" s="5">
         <v>2970</v>
       </c>
-      <c r="J72" s="18">
+      <c r="J72" s="16">
         <f t="shared" si="1"/>
         <v>164416</v>
       </c>
@@ -3617,7 +3800,7 @@
       <c r="I73" s="4">
         <v>3102</v>
       </c>
-      <c r="J73" s="18">
+      <c r="J73" s="16">
         <f t="shared" si="1"/>
         <v>172640</v>
       </c>
@@ -3650,7 +3833,7 @@
       <c r="I74" s="5">
         <v>857</v>
       </c>
-      <c r="J74" s="18">
+      <c r="J74" s="16">
         <f t="shared" si="1"/>
         <v>128058</v>
       </c>
@@ -3683,7 +3866,7 @@
       <c r="I75" s="4">
         <v>1357</v>
       </c>
-      <c r="J75" s="18">
+      <c r="J75" s="16">
         <f t="shared" si="1"/>
         <v>166119</v>
       </c>
@@ -3716,7 +3899,7 @@
       <c r="I76" s="5">
         <v>2173</v>
       </c>
-      <c r="J76" s="18">
+      <c r="J76" s="16">
         <f t="shared" si="1"/>
         <v>202415</v>
       </c>
@@ -3749,7 +3932,7 @@
       <c r="I77" s="4">
         <v>4192</v>
       </c>
-      <c r="J77" s="18">
+      <c r="J77" s="16">
         <f t="shared" si="1"/>
         <v>243431</v>
       </c>
@@ -3782,7 +3965,7 @@
       <c r="I78" s="5">
         <v>7806</v>
       </c>
-      <c r="J78" s="18">
+      <c r="J78" s="16">
         <f t="shared" si="1"/>
         <v>280923</v>
       </c>
@@ -3815,7 +3998,7 @@
       <c r="I79" s="4">
         <v>11544</v>
       </c>
-      <c r="J79" s="18">
+      <c r="J79" s="16">
         <f t="shared" si="1"/>
         <v>308980</v>
       </c>
@@ -3830,11 +4013,15 @@
       <c r="C80" s="5">
         <v>7800</v>
       </c>
-      <c r="D80" s="5"/>
+      <c r="D80" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E80" s="5">
         <v>5267</v>
       </c>
-      <c r="F80" s="5"/>
+      <c r="F80" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G80" s="5">
         <v>18</v>
       </c>
@@ -3844,7 +4031,7 @@
       <c r="I80" s="5">
         <v>4</v>
       </c>
-      <c r="J80" s="18">
+      <c r="J80" s="16">
         <f t="shared" si="1"/>
         <v>13116</v>
       </c>
@@ -3877,7 +4064,7 @@
       <c r="I81" s="4">
         <v>39</v>
       </c>
-      <c r="J81" s="18">
+      <c r="J81" s="16">
         <f t="shared" si="1"/>
         <v>15546</v>
       </c>
@@ -3910,7 +4097,7 @@
       <c r="I82" s="5">
         <v>13</v>
       </c>
-      <c r="J82" s="18">
+      <c r="J82" s="16">
         <f t="shared" si="1"/>
         <v>16846</v>
       </c>
@@ -3943,7 +4130,7 @@
       <c r="I83" s="4">
         <v>0</v>
       </c>
-      <c r="J83" s="18">
+      <c r="J83" s="16">
         <f t="shared" si="1"/>
         <v>16746</v>
       </c>
@@ -3976,7 +4163,7 @@
       <c r="I84" s="5">
         <v>0</v>
       </c>
-      <c r="J84" s="18">
+      <c r="J84" s="16">
         <f t="shared" si="1"/>
         <v>18783</v>
       </c>
@@ -4009,7 +4196,7 @@
       <c r="I85" s="4">
         <v>0</v>
       </c>
-      <c r="J85" s="18">
+      <c r="J85" s="16">
         <f t="shared" si="1"/>
         <v>19897</v>
       </c>
@@ -4033,14 +4220,16 @@
       <c r="F86" s="5">
         <v>530</v>
       </c>
-      <c r="G86" s="5"/>
+      <c r="G86" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H86" s="5">
         <v>5248</v>
       </c>
       <c r="I86" s="5">
         <v>2636</v>
       </c>
-      <c r="J86" s="18">
+      <c r="J86" s="16">
         <f t="shared" si="1"/>
         <v>421964</v>
       </c>
@@ -4064,14 +4253,16 @@
       <c r="F87" s="4">
         <v>3223</v>
       </c>
-      <c r="G87" s="4"/>
+      <c r="G87" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="H87" s="4">
         <v>7135</v>
       </c>
       <c r="I87" s="4">
         <v>2912</v>
       </c>
-      <c r="J87" s="18">
+      <c r="J87" s="16">
         <f t="shared" si="1"/>
         <v>394702</v>
       </c>
@@ -4104,7 +4295,7 @@
       <c r="I88" s="5">
         <v>3197</v>
       </c>
-      <c r="J88" s="18">
+      <c r="J88" s="16">
         <f t="shared" si="1"/>
         <v>453164</v>
       </c>
@@ -4137,7 +4328,7 @@
       <c r="I89" s="4">
         <v>3989</v>
       </c>
-      <c r="J89" s="18">
+      <c r="J89" s="16">
         <f t="shared" si="1"/>
         <v>388022</v>
       </c>
@@ -4170,7 +4361,7 @@
       <c r="I90" s="5">
         <v>1</v>
       </c>
-      <c r="J90" s="18">
+      <c r="J90" s="16">
         <f t="shared" si="1"/>
         <v>424736</v>
       </c>
@@ -4182,14 +4373,28 @@
       <c r="B91" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
-      <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-      <c r="I91" s="4"/>
-      <c r="J91" s="18">
+      <c r="C91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J91" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4204,7 +4409,9 @@
       <c r="C92" s="5">
         <v>136689</v>
       </c>
-      <c r="D92" s="5"/>
+      <c r="D92" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E92" s="5">
         <v>181061</v>
       </c>
@@ -4217,8 +4424,10 @@
       <c r="H92" s="5">
         <v>1285</v>
       </c>
-      <c r="I92" s="5"/>
-      <c r="J92" s="18">
+      <c r="I92" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J92" s="16">
         <f t="shared" si="1"/>
         <v>320144</v>
       </c>
@@ -4233,7 +4442,9 @@
       <c r="C93" s="4">
         <v>128670</v>
       </c>
-      <c r="D93" s="4"/>
+      <c r="D93" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E93" s="4">
         <v>172574</v>
       </c>
@@ -4246,8 +4457,10 @@
       <c r="H93" s="4">
         <v>2074</v>
       </c>
-      <c r="I93" s="4"/>
-      <c r="J93" s="18">
+      <c r="I93" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J93" s="16">
         <f t="shared" si="1"/>
         <v>304878</v>
       </c>
@@ -4280,7 +4493,7 @@
       <c r="I94" s="5">
         <v>0</v>
       </c>
-      <c r="J94" s="18">
+      <c r="J94" s="16">
         <f t="shared" si="1"/>
         <v>310399</v>
       </c>
@@ -4313,7 +4526,7 @@
       <c r="I95" s="4">
         <v>0</v>
       </c>
-      <c r="J95" s="18">
+      <c r="J95" s="16">
         <f t="shared" si="1"/>
         <v>333549</v>
       </c>
@@ -4328,7 +4541,9 @@
       <c r="C96" s="5">
         <v>171862</v>
       </c>
-      <c r="D96" s="5"/>
+      <c r="D96" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E96" s="5">
         <v>175590</v>
       </c>
@@ -4344,7 +4559,7 @@
       <c r="I96" s="5">
         <v>0</v>
       </c>
-      <c r="J96" s="18">
+      <c r="J96" s="16">
         <f t="shared" si="1"/>
         <v>358867</v>
       </c>
@@ -4377,7 +4592,7 @@
       <c r="I97" s="4">
         <v>0</v>
       </c>
-      <c r="J97" s="18">
+      <c r="J97" s="16">
         <f t="shared" si="1"/>
         <v>347935</v>
       </c>
@@ -4410,7 +4625,7 @@
       <c r="I98" s="5">
         <v>11</v>
       </c>
-      <c r="J98" s="18">
+      <c r="J98" s="16">
         <f t="shared" si="1"/>
         <v>1057748</v>
       </c>
@@ -4443,7 +4658,7 @@
       <c r="I99" s="4">
         <v>19</v>
       </c>
-      <c r="J99" s="18">
+      <c r="J99" s="16">
         <f t="shared" si="1"/>
         <v>1121876</v>
       </c>
@@ -4476,7 +4691,7 @@
       <c r="I100" s="5">
         <v>20</v>
       </c>
-      <c r="J100" s="18">
+      <c r="J100" s="16">
         <f t="shared" si="1"/>
         <v>1238455</v>
       </c>
@@ -4509,7 +4724,7 @@
       <c r="I101" s="4">
         <v>24</v>
       </c>
-      <c r="J101" s="18">
+      <c r="J101" s="16">
         <f t="shared" si="1"/>
         <v>1473005</v>
       </c>
@@ -4542,7 +4757,7 @@
       <c r="I102" s="5">
         <v>33</v>
       </c>
-      <c r="J102" s="18">
+      <c r="J102" s="16">
         <f t="shared" si="1"/>
         <v>1453688</v>
       </c>
@@ -4554,14 +4769,28 @@
       <c r="B103" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
-      <c r="F103" s="4"/>
-      <c r="G103" s="4"/>
-      <c r="H103" s="4"/>
-      <c r="I103" s="4"/>
-      <c r="J103" s="18">
+      <c r="C103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J103" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4573,14 +4802,28 @@
       <c r="B104" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="5"/>
-      <c r="G104" s="5"/>
-      <c r="H104" s="5"/>
-      <c r="I104" s="5"/>
-      <c r="J104" s="18">
+      <c r="C104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J104" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4592,14 +4835,28 @@
       <c r="B105" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C105" s="4"/>
-      <c r="D105" s="4"/>
-      <c r="E105" s="4"/>
-      <c r="F105" s="4"/>
-      <c r="G105" s="4"/>
-      <c r="H105" s="4"/>
-      <c r="I105" s="4"/>
-      <c r="J105" s="18">
+      <c r="C105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I105" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J105" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4611,14 +4868,28 @@
       <c r="B106" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
-      <c r="H106" s="5"/>
-      <c r="I106" s="5"/>
-      <c r="J106" s="18">
+      <c r="C106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J106" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4630,14 +4901,28 @@
       <c r="B107" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C107" s="4"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
-      <c r="F107" s="4"/>
-      <c r="G107" s="4"/>
-      <c r="H107" s="4"/>
-      <c r="I107" s="4"/>
-      <c r="J107" s="18">
+      <c r="C107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J107" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4670,7 +4955,7 @@
       <c r="I108" s="5">
         <v>68180</v>
       </c>
-      <c r="J108" s="18">
+      <c r="J108" s="16">
         <f t="shared" si="1"/>
         <v>364103</v>
       </c>
@@ -4703,7 +4988,7 @@
       <c r="I109" s="4">
         <v>77594</v>
       </c>
-      <c r="J109" s="18">
+      <c r="J109" s="16">
         <f t="shared" si="1"/>
         <v>389664</v>
       </c>
@@ -4736,7 +5021,7 @@
       <c r="I110" s="5">
         <v>1</v>
       </c>
-      <c r="J110" s="18">
+      <c r="J110" s="16">
         <f t="shared" si="1"/>
         <v>58302</v>
       </c>
@@ -4766,8 +5051,10 @@
       <c r="H111" s="4">
         <v>1039</v>
       </c>
-      <c r="I111" s="4"/>
-      <c r="J111" s="18">
+      <c r="I111" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J111" s="16">
         <f t="shared" si="1"/>
         <v>71214</v>
       </c>
@@ -4797,8 +5084,10 @@
       <c r="H112" s="5">
         <v>1213</v>
       </c>
-      <c r="I112" s="5"/>
-      <c r="J112" s="18">
+      <c r="I112" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J112" s="16">
         <f t="shared" si="1"/>
         <v>82388</v>
       </c>
@@ -4828,8 +5117,10 @@
       <c r="H113" s="4">
         <v>2168</v>
       </c>
-      <c r="I113" s="4"/>
-      <c r="J113" s="18">
+      <c r="I113" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J113" s="16">
         <f t="shared" si="1"/>
         <v>97349</v>
       </c>
@@ -4862,7 +5153,7 @@
       <c r="I114" s="5">
         <v>1</v>
       </c>
-      <c r="J114" s="18">
+      <c r="J114" s="16">
         <f t="shared" si="1"/>
         <v>110103</v>
       </c>
@@ -4883,15 +5174,19 @@
       <c r="E115" s="4">
         <v>53239</v>
       </c>
-      <c r="F115" s="4"/>
+      <c r="F115" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G115" s="4">
         <v>4449</v>
       </c>
       <c r="H115" s="4">
         <v>5809</v>
       </c>
-      <c r="I115" s="4"/>
-      <c r="J115" s="18">
+      <c r="I115" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J115" s="16">
         <f t="shared" si="1"/>
         <v>136730</v>
       </c>
@@ -4906,17 +5201,25 @@
       <c r="C116" s="5">
         <v>23942</v>
       </c>
-      <c r="D116" s="5"/>
+      <c r="D116" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E116" s="5">
         <v>28016</v>
       </c>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
+      <c r="F116" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G116" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H116" s="5">
         <v>10</v>
       </c>
-      <c r="I116" s="5"/>
-      <c r="J116" s="18">
+      <c r="I116" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J116" s="16">
         <f t="shared" si="1"/>
         <v>51968</v>
       </c>
@@ -4949,7 +5252,7 @@
       <c r="I117" s="4">
         <v>113</v>
       </c>
-      <c r="J117" s="18">
+      <c r="J117" s="16">
         <f t="shared" si="1"/>
         <v>41203</v>
       </c>
@@ -4982,7 +5285,7 @@
       <c r="I118" s="5">
         <v>237</v>
       </c>
-      <c r="J118" s="18">
+      <c r="J118" s="16">
         <f t="shared" si="1"/>
         <v>61267</v>
       </c>
@@ -5015,7 +5318,7 @@
       <c r="I119" s="4">
         <v>431</v>
       </c>
-      <c r="J119" s="18">
+      <c r="J119" s="16">
         <f t="shared" si="1"/>
         <v>65780</v>
       </c>
@@ -5048,7 +5351,7 @@
       <c r="I120" s="5">
         <v>1163</v>
       </c>
-      <c r="J120" s="18">
+      <c r="J120" s="16">
         <f t="shared" si="1"/>
         <v>74315</v>
       </c>
@@ -5081,7 +5384,7 @@
       <c r="I121" s="4">
         <v>1719</v>
       </c>
-      <c r="J121" s="18">
+      <c r="J121" s="16">
         <f t="shared" si="1"/>
         <v>76919</v>
       </c>
@@ -5114,7 +5417,7 @@
       <c r="I122" s="5">
         <v>2</v>
       </c>
-      <c r="J122" s="18">
+      <c r="J122" s="16">
         <f t="shared" si="1"/>
         <v>102966</v>
       </c>
@@ -5147,7 +5450,7 @@
       <c r="I123" s="4">
         <v>0</v>
       </c>
-      <c r="J123" s="18">
+      <c r="J123" s="16">
         <f t="shared" si="1"/>
         <v>106455</v>
       </c>
@@ -5180,7 +5483,7 @@
       <c r="I124" s="5">
         <v>0</v>
       </c>
-      <c r="J124" s="18">
+      <c r="J124" s="16">
         <f t="shared" si="1"/>
         <v>109080</v>
       </c>
@@ -5213,7 +5516,7 @@
       <c r="I125" s="4">
         <v>0</v>
       </c>
-      <c r="J125" s="18">
+      <c r="J125" s="16">
         <f t="shared" si="1"/>
         <v>119261</v>
       </c>
@@ -5246,7 +5549,7 @@
       <c r="I126" s="5">
         <v>0</v>
       </c>
-      <c r="J126" s="18">
+      <c r="J126" s="16">
         <f t="shared" si="1"/>
         <v>119154</v>
       </c>
@@ -5279,7 +5582,7 @@
       <c r="I127" s="4">
         <v>0</v>
       </c>
-      <c r="J127" s="18">
+      <c r="J127" s="16">
         <f t="shared" si="1"/>
         <v>121463</v>
       </c>
@@ -5312,7 +5615,7 @@
       <c r="I128" s="5">
         <v>3281</v>
       </c>
-      <c r="J128" s="18">
+      <c r="J128" s="16">
         <f t="shared" si="1"/>
         <v>297221</v>
       </c>
@@ -5327,7 +5630,9 @@
       <c r="C129" s="4">
         <v>126019</v>
       </c>
-      <c r="D129" s="4"/>
+      <c r="D129" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E129" s="4">
         <v>188998</v>
       </c>
@@ -5343,7 +5648,7 @@
       <c r="I129" s="4">
         <v>2722</v>
       </c>
-      <c r="J129" s="18">
+      <c r="J129" s="16">
         <f t="shared" si="1"/>
         <v>329620</v>
       </c>
@@ -5376,7 +5681,7 @@
       <c r="I130" s="5">
         <v>1396</v>
       </c>
-      <c r="J130" s="18">
+      <c r="J130" s="16">
         <f t="shared" si="1"/>
         <v>367106</v>
       </c>
@@ -5409,7 +5714,7 @@
       <c r="I131" s="4">
         <v>888</v>
       </c>
-      <c r="J131" s="18">
+      <c r="J131" s="16">
         <f t="shared" ref="J131:J175" si="2">SUM(C131:I131)</f>
         <v>392377</v>
       </c>
@@ -5442,7 +5747,7 @@
       <c r="I132" s="5">
         <v>1133</v>
       </c>
-      <c r="J132" s="18">
+      <c r="J132" s="16">
         <f t="shared" si="2"/>
         <v>398989</v>
       </c>
@@ -5475,7 +5780,7 @@
       <c r="I133" s="4">
         <v>1043</v>
       </c>
-      <c r="J133" s="18">
+      <c r="J133" s="16">
         <f t="shared" si="2"/>
         <v>374295</v>
       </c>
@@ -5487,14 +5792,28 @@
       <c r="B134" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
-      <c r="E134" s="5"/>
-      <c r="F134" s="5"/>
-      <c r="G134" s="5"/>
-      <c r="H134" s="5"/>
-      <c r="I134" s="5"/>
-      <c r="J134" s="18">
+      <c r="C134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J134" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5506,14 +5825,28 @@
       <c r="B135" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C135" s="4"/>
-      <c r="D135" s="4"/>
-      <c r="E135" s="4"/>
-      <c r="F135" s="4"/>
-      <c r="G135" s="4"/>
-      <c r="H135" s="4"/>
-      <c r="I135" s="4"/>
-      <c r="J135" s="18">
+      <c r="C135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I135" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J135" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5528,7 +5861,9 @@
       <c r="C136" s="5">
         <v>1334875</v>
       </c>
-      <c r="D136" s="5"/>
+      <c r="D136" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E136" s="5">
         <v>1257152</v>
       </c>
@@ -5544,7 +5879,7 @@
       <c r="I136" s="5">
         <v>10</v>
       </c>
-      <c r="J136" s="18">
+      <c r="J136" s="16">
         <f t="shared" si="2"/>
         <v>2612232</v>
       </c>
@@ -5559,7 +5894,9 @@
       <c r="C137" s="4">
         <v>1390355</v>
       </c>
-      <c r="D137" s="4"/>
+      <c r="D137" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E137" s="4">
         <v>1264307</v>
       </c>
@@ -5575,7 +5912,7 @@
       <c r="I137" s="4">
         <v>2</v>
       </c>
-      <c r="J137" s="18">
+      <c r="J137" s="16">
         <f t="shared" si="2"/>
         <v>2675830</v>
       </c>
@@ -5590,7 +5927,9 @@
       <c r="C138" s="5">
         <v>1446500</v>
       </c>
-      <c r="D138" s="5"/>
+      <c r="D138" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E138" s="5">
         <v>1049086</v>
       </c>
@@ -5606,7 +5945,7 @@
       <c r="I138" s="5">
         <v>3</v>
       </c>
-      <c r="J138" s="18">
+      <c r="J138" s="16">
         <f t="shared" si="2"/>
         <v>2523063</v>
       </c>
@@ -5621,7 +5960,9 @@
       <c r="C139" s="4">
         <v>1589618</v>
       </c>
-      <c r="D139" s="4"/>
+      <c r="D139" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E139" s="4">
         <v>736172</v>
       </c>
@@ -5637,7 +5978,7 @@
       <c r="I139" s="4">
         <v>3</v>
       </c>
-      <c r="J139" s="18">
+      <c r="J139" s="16">
         <f t="shared" si="2"/>
         <v>2357088</v>
       </c>
@@ -5670,7 +6011,7 @@
       <c r="I140" s="5">
         <v>0</v>
       </c>
-      <c r="J140" s="18">
+      <c r="J140" s="16">
         <f t="shared" si="2"/>
         <v>1938</v>
       </c>
@@ -5703,7 +6044,7 @@
       <c r="I141" s="4">
         <v>0</v>
       </c>
-      <c r="J141" s="18">
+      <c r="J141" s="16">
         <f t="shared" si="2"/>
         <v>1819</v>
       </c>
@@ -5736,7 +6077,7 @@
       <c r="I142" s="5">
         <v>0</v>
       </c>
-      <c r="J142" s="18">
+      <c r="J142" s="16">
         <f t="shared" si="2"/>
         <v>2084</v>
       </c>
@@ -5769,7 +6110,7 @@
       <c r="I143" s="4">
         <v>0</v>
       </c>
-      <c r="J143" s="18">
+      <c r="J143" s="16">
         <f t="shared" si="2"/>
         <v>2031</v>
       </c>
@@ -5802,7 +6143,7 @@
       <c r="I144" s="5">
         <v>0</v>
       </c>
-      <c r="J144" s="18">
+      <c r="J144" s="16">
         <f t="shared" si="2"/>
         <v>2082</v>
       </c>
@@ -5835,7 +6176,7 @@
       <c r="I145" s="4">
         <v>0</v>
       </c>
-      <c r="J145" s="18">
+      <c r="J145" s="16">
         <f t="shared" si="2"/>
         <v>1898</v>
       </c>
@@ -5850,11 +6191,15 @@
       <c r="C146" s="5">
         <v>67701</v>
       </c>
-      <c r="D146" s="5"/>
+      <c r="D146" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E146" s="5">
         <v>97464</v>
       </c>
-      <c r="F146" s="5"/>
+      <c r="F146" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G146" s="5">
         <v>9970</v>
       </c>
@@ -5864,7 +6209,7 @@
       <c r="I146" s="5">
         <v>884</v>
       </c>
-      <c r="J146" s="18">
+      <c r="J146" s="16">
         <f t="shared" si="2"/>
         <v>186603</v>
       </c>
@@ -5879,11 +6224,15 @@
       <c r="C147" s="4">
         <v>62997</v>
       </c>
-      <c r="D147" s="4"/>
+      <c r="D147" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E147" s="4">
         <v>87738</v>
       </c>
-      <c r="F147" s="4"/>
+      <c r="F147" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G147" s="4">
         <v>21153</v>
       </c>
@@ -5893,7 +6242,7 @@
       <c r="I147" s="4">
         <v>154</v>
       </c>
-      <c r="J147" s="18">
+      <c r="J147" s="16">
         <f t="shared" si="2"/>
         <v>193349</v>
       </c>
@@ -5908,11 +6257,15 @@
       <c r="C148" s="5">
         <v>64686</v>
       </c>
-      <c r="D148" s="5"/>
+      <c r="D148" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E148" s="5">
         <v>89499</v>
       </c>
-      <c r="F148" s="5"/>
+      <c r="F148" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G148" s="5">
         <v>21997</v>
       </c>
@@ -5922,7 +6275,7 @@
       <c r="I148" s="5">
         <v>154</v>
       </c>
-      <c r="J148" s="18">
+      <c r="J148" s="16">
         <f t="shared" si="2"/>
         <v>198487</v>
       </c>
@@ -5937,7 +6290,9 @@
       <c r="C149" s="4">
         <v>86537</v>
       </c>
-      <c r="D149" s="4"/>
+      <c r="D149" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="E149" s="4">
         <v>56095</v>
       </c>
@@ -5953,7 +6308,7 @@
       <c r="I149" s="4">
         <v>8</v>
       </c>
-      <c r="J149" s="18">
+      <c r="J149" s="16">
         <f t="shared" si="2"/>
         <v>200611</v>
       </c>
@@ -5968,7 +6323,9 @@
       <c r="C150" s="5">
         <v>95077</v>
       </c>
-      <c r="D150" s="5"/>
+      <c r="D150" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="E150" s="5">
         <v>46970</v>
       </c>
@@ -5984,7 +6341,7 @@
       <c r="I150" s="5">
         <v>5</v>
       </c>
-      <c r="J150" s="18">
+      <c r="J150" s="16">
         <f t="shared" si="2"/>
         <v>225353</v>
       </c>
@@ -6017,7 +6374,7 @@
       <c r="I151" s="4">
         <v>8</v>
       </c>
-      <c r="J151" s="18">
+      <c r="J151" s="16">
         <f t="shared" si="2"/>
         <v>231945</v>
       </c>
@@ -6050,7 +6407,7 @@
       <c r="I152" s="5">
         <v>0</v>
       </c>
-      <c r="J152" s="18">
+      <c r="J152" s="16">
         <f t="shared" si="2"/>
         <v>312000</v>
       </c>
@@ -6083,7 +6440,7 @@
       <c r="I153" s="4">
         <v>100</v>
       </c>
-      <c r="J153" s="18">
+      <c r="J153" s="16">
         <f t="shared" si="2"/>
         <v>305500</v>
       </c>
@@ -6116,7 +6473,7 @@
       <c r="I154" s="5">
         <v>100</v>
       </c>
-      <c r="J154" s="18">
+      <c r="J154" s="16">
         <f t="shared" si="2"/>
         <v>331400</v>
       </c>
@@ -6149,7 +6506,7 @@
       <c r="I155" s="4">
         <v>100</v>
       </c>
-      <c r="J155" s="18">
+      <c r="J155" s="16">
         <f t="shared" si="2"/>
         <v>322500</v>
       </c>
@@ -6182,7 +6539,7 @@
       <c r="I156" s="5">
         <v>100</v>
       </c>
-      <c r="J156" s="18">
+      <c r="J156" s="16">
         <f t="shared" si="2"/>
         <v>320100</v>
       </c>
@@ -6215,14 +6572,14 @@
       <c r="I157" s="4">
         <v>0</v>
       </c>
-      <c r="J157" s="18">
+      <c r="J157" s="16">
         <f t="shared" si="2"/>
         <v>306400</v>
       </c>
     </row>
     <row r="158" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B158" s="3" t="s">
         <v>69</v>
@@ -6236,110 +6593,184 @@
       <c r="E158" s="5">
         <v>22778</v>
       </c>
-      <c r="F158" s="5"/>
-      <c r="G158" s="5"/>
+      <c r="F158" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="H158" s="5">
         <v>220</v>
       </c>
       <c r="I158" s="5">
         <v>61</v>
       </c>
-      <c r="J158" s="18">
+      <c r="J158" s="16">
         <f t="shared" si="2"/>
         <v>32147</v>
       </c>
     </row>
     <row r="159" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B159" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C159" s="4"/>
-      <c r="D159" s="4"/>
-      <c r="E159" s="4"/>
-      <c r="F159" s="4"/>
-      <c r="G159" s="4"/>
-      <c r="H159" s="4"/>
-      <c r="I159" s="4"/>
-      <c r="J159" s="18">
+      <c r="C159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I159" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J159" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B160" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C160" s="5"/>
-      <c r="D160" s="5"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
-      <c r="G160" s="5"/>
-      <c r="H160" s="5"/>
-      <c r="I160" s="5"/>
-      <c r="J160" s="18">
+      <c r="C160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I160" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J160" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B161" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C161" s="4"/>
-      <c r="D161" s="4"/>
-      <c r="E161" s="4"/>
-      <c r="F161" s="4"/>
-      <c r="G161" s="4"/>
-      <c r="H161" s="4"/>
-      <c r="I161" s="4"/>
-      <c r="J161" s="18">
+      <c r="C161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I161" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J161" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B162" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
-      <c r="E162" s="5"/>
-      <c r="F162" s="5"/>
-      <c r="G162" s="5"/>
-      <c r="H162" s="5"/>
-      <c r="I162" s="5"/>
-      <c r="J162" s="18">
+      <c r="C162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I162" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J162" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C163" s="4"/>
-      <c r="D163" s="4"/>
-      <c r="E163" s="4"/>
-      <c r="F163" s="4"/>
-      <c r="G163" s="4"/>
-      <c r="H163" s="4"/>
-      <c r="I163" s="4"/>
-      <c r="J163" s="18">
+      <c r="C163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I163" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J163" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -6369,8 +6800,10 @@
       <c r="H164" s="5">
         <v>14495</v>
       </c>
-      <c r="I164" s="5"/>
-      <c r="J164" s="18">
+      <c r="I164" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J164" s="16">
         <f t="shared" si="2"/>
         <v>669400</v>
       </c>
@@ -6400,8 +6833,10 @@
       <c r="H165" s="4">
         <v>11404</v>
       </c>
-      <c r="I165" s="4"/>
-      <c r="J165" s="18">
+      <c r="I165" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J165" s="16">
         <f t="shared" si="2"/>
         <v>597218</v>
       </c>
@@ -6422,15 +6857,19 @@
       <c r="E166" s="5">
         <v>462191</v>
       </c>
-      <c r="F166" s="5"/>
+      <c r="F166" s="5" t="s">
+        <v>82</v>
+      </c>
       <c r="G166" s="5">
         <v>154</v>
       </c>
       <c r="H166" s="5">
         <v>13442</v>
       </c>
-      <c r="I166" s="5"/>
-      <c r="J166" s="18">
+      <c r="I166" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J166" s="16">
         <f t="shared" si="2"/>
         <v>759837</v>
       </c>
@@ -6451,15 +6890,19 @@
       <c r="E167" s="4">
         <v>460829</v>
       </c>
-      <c r="F167" s="4"/>
+      <c r="F167" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="G167" s="4">
         <v>77</v>
       </c>
       <c r="H167" s="4">
         <v>13792</v>
       </c>
-      <c r="I167" s="4"/>
-      <c r="J167" s="18">
+      <c r="I167" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J167" s="16">
         <f t="shared" si="2"/>
         <v>759866</v>
       </c>
@@ -6492,7 +6935,7 @@
       <c r="I168" s="5">
         <v>0</v>
       </c>
-      <c r="J168" s="18">
+      <c r="J168" s="16">
         <f t="shared" si="2"/>
         <v>767410</v>
       </c>
@@ -6525,90 +6968,146 @@
       <c r="I169" s="4">
         <v>0</v>
       </c>
-      <c r="J169" s="18">
+      <c r="J169" s="16">
         <f t="shared" si="2"/>
         <v>552887</v>
       </c>
     </row>
     <row r="170" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B170" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C170" s="5"/>
-      <c r="D170" s="5"/>
-      <c r="E170" s="5"/>
-      <c r="F170" s="5"/>
-      <c r="G170" s="5"/>
-      <c r="H170" s="5"/>
-      <c r="I170" s="5"/>
-      <c r="J170" s="18">
+      <c r="C170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J170" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B171" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C171" s="4"/>
-      <c r="D171" s="4"/>
-      <c r="E171" s="4"/>
-      <c r="F171" s="4"/>
-      <c r="G171" s="4"/>
-      <c r="H171" s="4"/>
-      <c r="I171" s="4"/>
-      <c r="J171" s="18">
+      <c r="C171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I171" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J171" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C172" s="5"/>
-      <c r="D172" s="5"/>
-      <c r="E172" s="5"/>
-      <c r="F172" s="5"/>
-      <c r="G172" s="5"/>
-      <c r="H172" s="5"/>
-      <c r="I172" s="5"/>
-      <c r="J172" s="18">
+      <c r="C172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I172" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J172" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B173" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C173" s="4"/>
-      <c r="D173" s="4"/>
-      <c r="E173" s="4"/>
-      <c r="F173" s="4"/>
-      <c r="G173" s="4"/>
-      <c r="H173" s="4"/>
-      <c r="I173" s="4"/>
-      <c r="J173" s="18">
+      <c r="C173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I173" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J173" s="16">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>73</v>
@@ -6634,14 +7133,14 @@
       <c r="I174" s="5">
         <v>2</v>
       </c>
-      <c r="J174" s="18">
+      <c r="J174" s="16">
         <f t="shared" si="2"/>
         <v>19504</v>
       </c>
     </row>
     <row r="175" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="B175" s="3" t="s">
         <v>74</v>
@@ -6667,24 +7166,10 @@
       <c r="I175" s="4">
         <v>0</v>
       </c>
-      <c r="J175" s="18">
+      <c r="J175" s="16">
         <f t="shared" si="2"/>
         <v>9843</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="178" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A178" s="1"/>
-      <c r="B178" s="2"/>
-    </row>
-    <row r="179" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A179" s="1"/>
-    </row>
-    <row r="180" spans="1:2" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A180" s="1"/>
-      <c r="B180" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>